<commit_message>
Don't subtract mgmt fee when deposit/redeem.
</commit_message>
<xml_diff>
--- a/contracts/vault/tests/files/Mars - 3rd party Vault - Performance Fee - test cases v1.0.xlsx
+++ b/contracts/vault/tests/files/Mars - 3rd party Vault - Performance Fee - test cases v1.0.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Annualized</t>
   </si>
@@ -29,9 +29,6 @@
     <t>(Manually insert these to simulate)</t>
   </si>
   <si>
-    <t>(Includes Mgr Fee)</t>
-  </si>
-  <si>
     <t>(If Deposit)</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Cum Mgr Fee</t>
   </si>
   <si>
-    <t>Share Price</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
   </si>
   <si>
     <t>Withdraw $ Amt</t>
-  </si>
-  <si>
-    <t>Before Action</t>
   </si>
   <si>
     <t>Post Vault Lqdty</t>
@@ -108,14 +99,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.00000%"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000000000%"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy h:mm"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000000%"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.000000%"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -186,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -232,26 +222,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="46" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -262,8 +246,8 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="169" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="170" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="169" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -493,15 +477,14 @@
     <col customWidth="1" min="5" max="5" width="15.88"/>
     <col customWidth="1" min="6" max="7" width="17.13"/>
     <col customWidth="1" min="8" max="8" width="15.38"/>
-    <col customWidth="1" min="9" max="9" width="15.0"/>
-    <col customWidth="1" min="10" max="10" width="26.38"/>
-    <col customWidth="1" min="11" max="11" width="13.5"/>
-    <col customWidth="1" min="12" max="12" width="18.13"/>
-    <col customWidth="1" min="13" max="13" width="20.88"/>
-    <col customWidth="1" min="14" max="15" width="15.38"/>
-    <col customWidth="1" min="16" max="16" width="20.0"/>
-    <col customWidth="1" min="17" max="17" width="21.88"/>
-    <col customWidth="1" min="18" max="18" width="15.13"/>
+    <col customWidth="1" min="9" max="9" width="26.38"/>
+    <col customWidth="1" min="10" max="10" width="13.5"/>
+    <col customWidth="1" min="11" max="11" width="18.13"/>
+    <col customWidth="1" min="12" max="12" width="20.88"/>
+    <col customWidth="1" min="13" max="13" width="15.38"/>
+    <col customWidth="1" min="14" max="14" width="20.0"/>
+    <col customWidth="1" min="15" max="15" width="21.88"/>
+    <col customWidth="1" min="16" max="16" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -558,74 +541,64 @@
         <v>4</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>4</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="11">
@@ -652,41 +625,34 @@
       <c r="H7" s="13">
         <v>0.0</v>
       </c>
-      <c r="I7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="12">
+      <c r="I7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="12">
         <v>1.0E8</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="17">
-        <f>K7*1000000</f>
+      <c r="K7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="16">
+        <f>J7*1000000</f>
         <v>100000000000000</v>
       </c>
+      <c r="M7" s="16">
+        <f t="shared" ref="M7:M13" si="3">IF(I7="Burn",FLOOR((B7-H7)*K7/C7,1),0)</f>
+        <v>0</v>
+      </c>
       <c r="N7" s="17">
-        <f t="shared" ref="N7:N13" si="3">IF(J7="Burn",FLOOR((B7-H7)*L7/C7,1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="18">
-        <f t="shared" ref="O7:O13" si="4">B7-H7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="19">
-        <f>K7</f>
+        <f>J7</f>
         <v>100000000</v>
       </c>
-      <c r="Q7" s="19">
-        <f t="shared" ref="Q7:Q13" si="5">IF(J7="Deposit",M7+C7,C7-L7)</f>
+      <c r="O7" s="17">
+        <f t="shared" ref="O7:O13" si="4">IF(I7="Deposit",L7+C7,C7-K7)</f>
         <v>100000000000000</v>
       </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="11">
@@ -695,60 +661,52 @@
       <c r="B8" s="12">
         <v>1.2E8</v>
       </c>
-      <c r="C8" s="19">
-        <f t="shared" ref="C8:C11" si="6">Q7</f>
+      <c r="C8" s="17">
+        <f t="shared" ref="C8:C11" si="5">O7</f>
         <v>100000000000000</v>
       </c>
       <c r="D8" s="18">
-        <f t="shared" ref="D8:D11" si="7">D7+(B8-P7)</f>
+        <f t="shared" ref="D8:D11" si="6">D7+(B8-N7)</f>
         <v>20000000</v>
       </c>
-      <c r="E8" s="20" t="str">
-        <f t="shared" ref="E8:E13" si="8">TEXT(A8-A7,"[H]")</f>
+      <c r="E8" s="19" t="str">
+        <f t="shared" ref="E8:E13" si="7">TEXT(A8-A7,"[H]")</f>
         <v>97</v>
       </c>
       <c r="F8" s="13">
-        <f t="shared" ref="F8:F11" si="9">F7+E8</f>
+        <f t="shared" ref="F8:F11" si="8">F7+E8</f>
         <v>97</v>
       </c>
       <c r="G8" s="14">
         <v>2.08E-5</v>
       </c>
-      <c r="H8" s="19">
-        <f t="shared" ref="H8:H13" si="10">FLOOR(IF(D8&gt;0,F8*G8*D8,0),1)</f>
+      <c r="H8" s="17">
+        <f t="shared" ref="H8:H13" si="9">FLOOR(IF(D8&gt;0,F8*G8*D8,0),1)</f>
         <v>40352</v>
       </c>
-      <c r="I8" s="21">
-        <f t="shared" ref="I8:I13" si="11">(B8-H8)/C8</f>
-        <v>0.00000119959648</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="12">
+      <c r="I8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12">
         <v>2.0E7</v>
       </c>
-      <c r="L8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="17">
-        <f t="shared" ref="M8:M13" si="12">IF(J8="Deposit",C8*K8/(B8-H8),0)</f>
+      <c r="K8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="16">
+        <f t="shared" ref="L8:L13" si="10">IF(I8="Deposit",C8*J8/(B8-H8),0)</f>
         <v>16672272996333</v>
       </c>
+      <c r="M8" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="N8" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="18">
+        <f t="shared" ref="N8:N10" si="11">IF(I8="Deposit",B8+J8,B8-M8)</f>
+        <v>140000000</v>
+      </c>
+      <c r="O8" s="17">
         <f t="shared" si="4"/>
-        <v>119959648</v>
-      </c>
-      <c r="P8" s="19">
-        <f t="shared" ref="P8:P10" si="13">IF(J8="Deposit",B8-H8+K8,B8-H8-N8)</f>
-        <v>139959648</v>
-      </c>
-      <c r="Q8" s="19">
-        <f t="shared" si="5"/>
         <v>116672272996333</v>
       </c>
     </row>
@@ -759,60 +717,52 @@
       <c r="B9" s="12">
         <v>6.0E7</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
+        <f t="shared" si="5"/>
+        <v>116672272996333</v>
+      </c>
+      <c r="D9" s="18">
         <f t="shared" si="6"/>
-        <v>116672272996333</v>
-      </c>
-      <c r="D9" s="18">
+        <v>-60000000</v>
+      </c>
+      <c r="E9" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>-59959648</v>
-      </c>
-      <c r="E9" s="20" t="str">
+        <v>72</v>
+      </c>
+      <c r="F9" s="13">
         <f t="shared" si="8"/>
-        <v>72</v>
-      </c>
-      <c r="F9" s="13">
-        <f t="shared" si="9"/>
         <v>169</v>
       </c>
       <c r="G9" s="14">
         <v>2.08E-5</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1.5E7</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="21">
+        <v>29168068249083</v>
+      </c>
+      <c r="M9" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
         <f t="shared" si="11"/>
-        <v>0.0000005142610019</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="12">
-        <v>1.5E7</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="17">
-        <f t="shared" si="12"/>
-        <v>29168068249083</v>
-      </c>
-      <c r="N9" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="18">
+        <v>75000000</v>
+      </c>
+      <c r="O9" s="17">
         <f t="shared" si="4"/>
-        <v>60000000</v>
-      </c>
-      <c r="P9" s="19">
-        <f t="shared" si="13"/>
-        <v>75000000</v>
-      </c>
-      <c r="Q9" s="19">
-        <f t="shared" si="5"/>
         <v>145840341245416</v>
       </c>
     </row>
@@ -823,60 +773,52 @@
       <c r="B10" s="12">
         <v>4.5E8</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="17">
+        <f t="shared" si="5"/>
+        <v>145840341245416</v>
+      </c>
+      <c r="D10" s="18">
         <f t="shared" si="6"/>
-        <v>145840341245416</v>
-      </c>
-      <c r="D10" s="18">
+        <v>315000000</v>
+      </c>
+      <c r="E10" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>315040352</v>
-      </c>
-      <c r="E10" s="20" t="str">
+        <v>144</v>
+      </c>
+      <c r="F10" s="13">
         <f t="shared" si="8"/>
-        <v>144</v>
-      </c>
-      <c r="F10" s="13">
-        <f t="shared" si="9"/>
         <v>313</v>
       </c>
       <c r="G10" s="14">
         <v>2.08E-5</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="17">
+        <f t="shared" si="9"/>
+        <v>2050776</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1.0E13</v>
+      </c>
+      <c r="L10" s="16">
         <f t="shared" si="10"/>
-        <v>2051038</v>
-      </c>
-      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="M10" s="16">
+        <f t="shared" si="3"/>
+        <v>30715042</v>
+      </c>
+      <c r="N10" s="17">
         <f t="shared" si="11"/>
-        <v>0.000003071502426</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="12">
-        <v>1.0E13</v>
-      </c>
-      <c r="M10" s="17">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="17">
-        <f t="shared" si="3"/>
-        <v>30715024</v>
-      </c>
-      <c r="O10" s="18">
+        <v>419284958</v>
+      </c>
+      <c r="O10" s="17">
         <f t="shared" si="4"/>
-        <v>447948962</v>
-      </c>
-      <c r="P10" s="19">
-        <f t="shared" si="13"/>
-        <v>417233938</v>
-      </c>
-      <c r="Q10" s="19">
-        <f t="shared" si="5"/>
         <v>135840341245416</v>
       </c>
     </row>
@@ -885,62 +827,54 @@
         <v>45396.63888888889</v>
       </c>
       <c r="B11" s="12">
-        <v>8.24284976E8</v>
-      </c>
-      <c r="C11" s="19">
+        <v>8.24284958E8</v>
+      </c>
+      <c r="C11" s="17">
+        <f t="shared" si="5"/>
+        <v>135840341245416</v>
+      </c>
+      <c r="D11" s="18">
         <f t="shared" si="6"/>
-        <v>135840341245416</v>
-      </c>
-      <c r="D11" s="18">
+        <v>720000000</v>
+      </c>
+      <c r="E11" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>722091390</v>
-      </c>
-      <c r="E11" s="20" t="str">
+        <v>744</v>
+      </c>
+      <c r="F11" s="13">
         <f t="shared" si="8"/>
-        <v>744</v>
-      </c>
-      <c r="F11" s="13">
-        <f t="shared" si="9"/>
         <v>1057</v>
       </c>
       <c r="G11" s="14">
         <v>2.08E-5</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="17">
+        <f t="shared" si="9"/>
+        <v>15829632</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="L11" s="16">
         <f t="shared" si="10"/>
-        <v>15875612</v>
-      </c>
-      <c r="I11" s="21">
-        <f t="shared" si="11"/>
-        <v>0.000005951172948</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="M11" s="17">
-        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="16">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="18">
+        <f>B11-H11</f>
+        <v>808455326</v>
+      </c>
+      <c r="O11" s="17">
         <f t="shared" si="4"/>
-        <v>808409364</v>
-      </c>
-      <c r="P11" s="19">
-        <f>B11-H11</f>
-        <v>808409364</v>
-      </c>
-      <c r="Q11" s="19">
-        <f t="shared" si="5"/>
         <v>135840341245416</v>
       </c>
     </row>
@@ -948,62 +882,54 @@
       <c r="A12" s="11">
         <v>45396.63888888889</v>
       </c>
-      <c r="B12" s="22">
-        <f t="shared" ref="B12:C12" si="14">P11</f>
-        <v>808409364</v>
-      </c>
-      <c r="C12" s="19">
-        <f t="shared" si="14"/>
+      <c r="B12" s="20">
+        <f t="shared" ref="B12:C12" si="12">N11</f>
+        <v>808455326</v>
+      </c>
+      <c r="C12" s="17">
+        <f t="shared" si="12"/>
         <v>135840341245416</v>
       </c>
-      <c r="D12" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="20" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="D12" s="20">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="19" t="str">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <v>0.0</v>
       </c>
       <c r="G12" s="14">
         <v>4.08E-5</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="L12" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I12" s="21">
-        <f t="shared" si="11"/>
-        <v>0.000005951172948</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="M12" s="17">
-        <f t="shared" si="12"/>
+      <c r="M12" s="16">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="18">
+        <f t="shared" ref="N12:N13" si="13">IF(I12="Deposit",B12+J12,B12-M12)</f>
+        <v>808455326</v>
+      </c>
+      <c r="O12" s="17">
         <f t="shared" si="4"/>
-        <v>808409364</v>
-      </c>
-      <c r="P12" s="19">
-        <f t="shared" ref="P12:P13" si="15">IF(J12="Deposit",B12-H12+K12,B12-H12-N12)</f>
-        <v>808409364</v>
-      </c>
-      <c r="Q12" s="19">
-        <f t="shared" si="5"/>
         <v>135840341245416</v>
       </c>
     </row>
@@ -1012,18 +938,18 @@
         <v>45398.63888888889</v>
       </c>
       <c r="B13" s="12">
-        <v>8.48409364E8</v>
-      </c>
-      <c r="C13" s="19">
-        <f>Q12</f>
+        <v>8.48455326E8</v>
+      </c>
+      <c r="C13" s="17">
+        <f>O12</f>
         <v>135840341245416</v>
       </c>
       <c r="D13" s="18">
-        <f>D12+(B13-P12)</f>
+        <f>D12+(B13-N12)</f>
         <v>40000000</v>
       </c>
-      <c r="E13" s="20" t="str">
-        <f t="shared" si="8"/>
+      <c r="E13" s="19" t="str">
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="F13" s="13">
@@ -1033,42 +959,34 @@
       <c r="G13" s="14">
         <v>4.08E-5</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="17">
+        <f t="shared" si="9"/>
+        <v>78336</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="12">
+        <v>5.5E7</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="16">
         <f t="shared" si="10"/>
-        <v>78336</v>
-      </c>
-      <c r="I13" s="21">
-        <f t="shared" si="11"/>
-        <v>0.000006245059606</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="12">
-        <v>5.5E7</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="17">
-        <f t="shared" si="12"/>
-        <v>8806961577383</v>
+        <v>8806484448026</v>
+      </c>
+      <c r="M13" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="N13" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="18">
+        <f t="shared" si="13"/>
+        <v>903455326</v>
+      </c>
+      <c r="O13" s="17">
         <f t="shared" si="4"/>
-        <v>848331028</v>
-      </c>
-      <c r="P13" s="19">
-        <f t="shared" si="15"/>
-        <v>903331028</v>
-      </c>
-      <c r="Q13" s="19">
-        <f t="shared" si="5"/>
-        <v>144647302822799</v>
+        <v>144646825693442</v>
       </c>
     </row>
     <row r="14">
@@ -1076,9 +994,9 @@
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15">
       <c r="A15" s="10"/>
@@ -1087,13 +1005,13 @@
       <c r="D15" s="10"/>
     </row>
     <row r="21">
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1116,15 +1034,14 @@
     <col customWidth="1" min="5" max="5" width="15.88"/>
     <col customWidth="1" min="6" max="7" width="17.13"/>
     <col customWidth="1" min="8" max="8" width="15.38"/>
-    <col customWidth="1" min="9" max="9" width="15.0"/>
-    <col customWidth="1" min="10" max="10" width="26.38"/>
-    <col customWidth="1" min="11" max="11" width="13.5"/>
-    <col customWidth="1" min="12" max="12" width="18.13"/>
-    <col customWidth="1" min="13" max="13" width="20.88"/>
-    <col customWidth="1" min="14" max="15" width="15.38"/>
-    <col customWidth="1" min="16" max="16" width="20.0"/>
-    <col customWidth="1" min="17" max="17" width="21.88"/>
-    <col customWidth="1" min="18" max="18" width="15.13"/>
+    <col customWidth="1" min="9" max="9" width="26.38"/>
+    <col customWidth="1" min="10" max="10" width="13.5"/>
+    <col customWidth="1" min="11" max="11" width="18.13"/>
+    <col customWidth="1" min="12" max="12" width="20.88"/>
+    <col customWidth="1" min="13" max="13" width="15.38"/>
+    <col customWidth="1" min="14" max="14" width="20.0"/>
+    <col customWidth="1" min="15" max="15" width="21.88"/>
+    <col customWidth="1" min="16" max="16" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1171,74 +1088,64 @@
         <v>4</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>4</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="11">
@@ -1265,41 +1172,34 @@
       <c r="H7" s="13">
         <v>0.0</v>
       </c>
-      <c r="I7" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="12">
+      <c r="I7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="12">
         <v>1.0E8</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="17">
-        <f>K7*1000000</f>
+      <c r="K7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="16">
+        <f>J7*1000000</f>
         <v>100000000000000</v>
       </c>
+      <c r="M7" s="16">
+        <f t="shared" ref="M7:M8" si="1">IF(I7="Burn",FLOOR((B7-H7)*K7/C7,1),0)</f>
+        <v>0</v>
+      </c>
       <c r="N7" s="17">
-        <f t="shared" ref="N7:N8" si="1">IF(J7="Burn",FLOOR((B7-H7)*L7/C7,1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="18">
-        <f t="shared" ref="O7:O8" si="2">B7-H7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="19">
-        <f>K7</f>
+        <f>J7</f>
         <v>100000000</v>
       </c>
-      <c r="Q7" s="19">
-        <f t="shared" ref="Q7:Q8" si="3">IF(J7="Deposit",M7+C7,C7-L7)</f>
+      <c r="O7" s="17">
+        <f t="shared" ref="O7:O8" si="2">IF(I7="Deposit",L7+C7,C7-K7)</f>
         <v>100000000000000</v>
       </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="11">
@@ -1308,15 +1208,15 @@
       <c r="B8" s="12">
         <v>1.2E8</v>
       </c>
-      <c r="C8" s="19">
-        <f>Q7</f>
+      <c r="C8" s="17">
+        <f>O7</f>
         <v>100000000000000</v>
       </c>
       <c r="D8" s="18">
-        <f>D7+(B8-P7)</f>
+        <f>D7+(B8-N7)</f>
         <v>20000000</v>
       </c>
-      <c r="E8" s="20" t="str">
+      <c r="E8" s="19" t="str">
         <f>TEXT(A8-A7,"[H]")</f>
         <v>2</v>
       </c>
@@ -1327,41 +1227,33 @@
       <c r="G8" s="14">
         <v>2.08E-5</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="17">
         <f>FLOOR(IF(D8&gt;0,F8*G8*D8,0),1)</f>
         <v>832</v>
       </c>
-      <c r="I8" s="21">
-        <f>(B8-H8)/C8</f>
-        <v>0.00000119999168</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>28</v>
+      <c r="I8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.0</v>
       </c>
       <c r="K8" s="12">
         <v>0.0</v>
       </c>
-      <c r="L8" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="M8" s="17">
-        <f>IF(J8="Deposit",C8*K8/(B8-H8),0)</f>
+      <c r="L8" s="16">
+        <f>IF(I8="Deposit",C8*J8/(B8-H8),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N8" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="18">
+        <f>B8-H8</f>
+        <v>119999168</v>
+      </c>
+      <c r="O8" s="17">
         <f t="shared" si="2"/>
-        <v>119999168</v>
-      </c>
-      <c r="P8" s="19">
-        <f>IF(J8="Deposit",B8-H8+K8,B8-H8-N8)</f>
-        <v>119999168</v>
-      </c>
-      <c r="Q8" s="19">
-        <f t="shared" si="3"/>
         <v>100000000000000</v>
       </c>
     </row>
@@ -1370,9 +1262,9 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10">
       <c r="A10" s="10"/>
@@ -1381,13 +1273,13 @@
       <c r="D10" s="10"/>
     </row>
     <row r="16">
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>